<commit_message>
Update Enhanced Data Files
</commit_message>
<xml_diff>
--- a/02_Enhanced Data/Data After Generation/Enhanced_dataset.xlsx
+++ b/02_Enhanced Data/Data After Generation/Enhanced_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\marwa\marwa\ITI\Grad. Project\02_Enhanced Data\Data After Generation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44E3A341-7FBC-467D-A19A-7632D01EB993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1952E9C-C8C7-4D87-9F03-920A2BEE3058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-2895" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19425" yWindow="-2130" windowWidth="17280" windowHeight="9795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Olist Normalized DB" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="99">
   <si>
     <t>Orders</t>
   </si>
@@ -316,18 +316,6 @@
     <t>No. Rows</t>
   </si>
   <si>
-    <t>Customer_City</t>
-  </si>
-  <si>
-    <t>Customer_State</t>
-  </si>
-  <si>
-    <t>Seller_City</t>
-  </si>
-  <si>
-    <t>Seller_State</t>
-  </si>
-  <si>
     <t>Olist Normalized DB</t>
   </si>
   <si>
@@ -356,9 +344,6 @@
   </si>
   <si>
     <t>No.Row:</t>
-  </si>
-  <si>
-    <t>company_id</t>
   </si>
 </sst>
 </file>
@@ -488,7 +473,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -688,11 +673,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -718,30 +712,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -759,22 +735,7 @@
       <alignment horizontal="left" indent="58"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -785,9 +746,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -800,12 +758,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -839,12 +791,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -854,10 +816,24 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1150,155 +1126,155 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C62CA94-1E60-47B9-AB4A-1DC4FE5D0C38}">
   <dimension ref="C2:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="20"/>
-    <col min="3" max="3" width="9" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="20"/>
-    <col min="7" max="7" width="9" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="20"/>
-    <col min="11" max="11" width="9" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="20"/>
-    <col min="15" max="15" width="8.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="20"/>
+    <col min="1" max="2" width="8.88671875" style="14"/>
+    <col min="3" max="3" width="9" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="14"/>
+    <col min="7" max="7" width="9" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="14"/>
+    <col min="11" max="11" width="9" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="14"/>
+    <col min="15" max="15" width="8.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.77734375" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="3:17" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="22"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
     </row>
     <row r="4" spans="3:17" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C4" s="22"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
     </row>
     <row r="5" spans="3:17" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="25"/>
-      <c r="D5" s="69" t="s">
+      <c r="C5" s="19"/>
+      <c r="D5" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
     </row>
     <row r="6" spans="3:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C7"/>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="55"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="32"/>
-      <c r="J7" s="55"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="41"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="32" t="s">
+      <c r="L7" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="M7" s="32"/>
-      <c r="N7" s="55"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="41"/>
     </row>
     <row r="8" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="48"/>
-      <c r="G8" s="40" t="s">
+      <c r="F8" s="34"/>
+      <c r="G8" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="30" t="s">
+      <c r="I8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="J8" s="48"/>
-      <c r="K8" s="11" t="s">
+      <c r="J8" s="34"/>
+      <c r="K8" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="L8" s="30" t="s">
+      <c r="L8" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="M8" s="30" t="s">
+      <c r="M8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N8" s="51"/>
+      <c r="N8" s="37"/>
     </row>
     <row r="9" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C9" s="6" t="s">
@@ -1307,11 +1283,11 @@
       <c r="D9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="48"/>
-      <c r="G9" s="41" t="s">
+      <c r="F9" s="34"/>
+      <c r="G9" s="29" t="s">
         <v>73</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -1320,8 +1296,8 @@
       <c r="I9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J9" s="48"/>
-      <c r="K9" s="17" t="s">
+      <c r="J9" s="34"/>
+      <c r="K9" s="57" t="s">
         <v>73</v>
       </c>
       <c r="L9" s="1" t="s">
@@ -1330,21 +1306,21 @@
       <c r="M9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
     </row>
     <row r="10" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C10" s="3"/>
       <c r="D10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="48"/>
-      <c r="G10" s="42" t="s">
+      <c r="F10" s="34"/>
+      <c r="G10" s="30" t="s">
         <v>83</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -1353,18 +1329,18 @@
       <c r="I10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J10" s="48"/>
-      <c r="K10" s="18"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="58"/>
       <c r="L10" s="1" t="s">
         <v>77</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
     </row>
     <row r="11" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C11" s="7" t="s">
@@ -1373,18 +1349,18 @@
       <c r="D11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="48"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="23" t="s">
+      <c r="F11" s="34"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="J11" s="48"/>
+      <c r="J11" s="34"/>
       <c r="K11" s="7" t="s">
         <v>75</v>
       </c>
@@ -1394,28 +1370,28 @@
       <c r="M11" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
     </row>
     <row r="12" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C12" s="3"/>
-      <c r="D12" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E12" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="49"/>
-      <c r="G12" s="44"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="35"/>
+      <c r="G12" s="32"/>
       <c r="H12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J12" s="49"/>
+      <c r="J12" s="35"/>
       <c r="K12" s="7" t="s">
         <v>75</v>
       </c>
@@ -1425,28 +1401,28 @@
       <c r="M12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
     </row>
     <row r="13" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C13" s="3"/>
-      <c r="D13" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E13" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="48"/>
-      <c r="G13" s="44"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="34"/>
+      <c r="G13" s="32"/>
       <c r="H13" s="9" t="s">
         <v>24</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J13" s="48"/>
+      <c r="J13" s="34"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1" t="s">
         <v>29</v>
@@ -1454,128 +1430,130 @@
       <c r="M13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
     </row>
     <row r="14" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
-      <c r="D14" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="48"/>
-      <c r="G14" s="44"/>
+      <c r="D14" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="34"/>
+      <c r="G14" s="32"/>
       <c r="H14" s="1" t="s">
         <v>25</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J14" s="48"/>
-      <c r="K14" s="36"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="25"/>
       <c r="L14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
     </row>
     <row r="15" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C15" s="1"/>
-      <c r="D15" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="48"/>
-      <c r="G15" s="44"/>
+      <c r="C15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="67">
+        <v>99441</v>
+      </c>
+      <c r="E15" s="68"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="32"/>
       <c r="H15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J15" s="48"/>
-      <c r="K15" s="36"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="25"/>
       <c r="L15" s="1" t="s">
         <v>31</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
     </row>
     <row r="16" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C16" s="1"/>
-      <c r="D16" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="48"/>
-      <c r="G16" s="44"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="32"/>
       <c r="H16" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J16" s="48"/>
-      <c r="K16" s="66" t="s">
+      <c r="J16" s="34"/>
+      <c r="K16" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="L16" s="34">
+      <c r="L16" s="56">
         <v>112650</v>
       </c>
-      <c r="M16" s="34"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
     </row>
     <row r="17" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C17" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" s="19">
-        <v>99441</v>
-      </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="62" t="s">
-        <v>103</v>
-      </c>
-      <c r="I17" s="62" t="s">
+      <c r="C17"/>
+      <c r="D17" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="59"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="J17" s="55"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
+      <c r="C18" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="15"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
         <v>28</v>
@@ -1583,61 +1561,63 @@
       <c r="I18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J18" s="55"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="15" t="s">
+      <c r="J18" s="41"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="M18" s="16"/>
-      <c r="N18" s="52"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
     </row>
     <row r="19" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C19"/>
-      <c r="D19" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="67" t="s">
+      <c r="C19" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="46"/>
+      <c r="G19" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="H19" s="68">
+      <c r="H19" s="65">
         <v>99441</v>
       </c>
-      <c r="I19" s="68"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="12" t="s">
+      <c r="I19" s="66"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="L19" s="12" t="s">
+      <c r="L19" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="M19" s="12" t="s">
+      <c r="M19" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="N19" s="51"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C20" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="55"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="60"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="41"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="46"/>
       <c r="K20" s="6" t="s">
         <v>73</v>
       </c>
@@ -1647,28 +1627,26 @@
       <c r="M20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N20" s="51"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
     </row>
     <row r="21" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C21" s="17" t="s">
-        <v>73</v>
-      </c>
+      <c r="C21" s="3"/>
       <c r="D21" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="55"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="41"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="I21" s="33"/>
-      <c r="J21" s="61"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="47"/>
       <c r="K21" s="7" t="s">
         <v>75</v>
       </c>
@@ -1678,52 +1656,52 @@
       <c r="M21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N21" s="53"/>
-      <c r="O21" s="56"/>
-      <c r="P21" s="56"/>
-      <c r="Q21" s="56"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="42"/>
+      <c r="P21" s="42"/>
+      <c r="Q21" s="42"/>
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C22" s="18"/>
+      <c r="C22" s="3"/>
       <c r="D22" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="48"/>
-      <c r="G22" s="45" t="s">
+      <c r="F22" s="34"/>
+      <c r="G22" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="H22" s="31" t="s">
+      <c r="H22" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="I22" s="31" t="s">
+      <c r="I22" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="J22" s="48"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="M22" s="1" t="s">
+      <c r="J22" s="34"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="M22" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="N22" s="51"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
     </row>
     <row r="23" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C23" s="3"/>
+      <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23" s="48"/>
-      <c r="G23" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="34"/>
+      <c r="G23" s="63" t="s">
         <v>73</v>
       </c>
       <c r="H23" s="1" t="s">
@@ -1732,370 +1710,362 @@
       <c r="I23" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J23" s="48"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N23" s="51"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="22"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="L23" s="56">
+        <v>3095</v>
+      </c>
+      <c r="M23" s="56"/>
+      <c r="N23" s="37"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
     </row>
     <row r="24" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C24" s="3"/>
-      <c r="D24" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="48"/>
-      <c r="G24" s="47"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="34"/>
+      <c r="G24" s="64"/>
       <c r="H24" s="1" t="s">
         <v>76</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J24" s="48"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="M24" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="N24" s="51"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="22"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="37"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
     </row>
     <row r="25" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C25" s="1"/>
-      <c r="D25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="F25" s="48"/>
-      <c r="G25" s="43"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="31"/>
       <c r="H25" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J25" s="48"/>
-      <c r="K25" s="66" t="s">
-        <v>88</v>
-      </c>
-      <c r="L25" s="34">
-        <v>3095</v>
-      </c>
-      <c r="M25" s="34"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="22"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="59" t="s">
+        <v>4</v>
+      </c>
+      <c r="M25" s="59"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
     </row>
     <row r="26" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C26" s="1"/>
-      <c r="D26" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="49"/>
-      <c r="G26" s="43"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="31"/>
       <c r="H26" s="1" t="s">
         <v>33</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="55"/>
-      <c r="M26" s="55"/>
-      <c r="N26" s="21"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="L26" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="M26" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="N26" s="15"/>
     </row>
     <row r="27" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="44"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="32"/>
       <c r="H27" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="73" t="s">
-        <v>4</v>
-      </c>
-      <c r="M27" s="73"/>
-      <c r="N27" s="55"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="M27" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="N27" s="41"/>
     </row>
     <row r="28" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="44"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="32"/>
       <c r="H28" s="1" t="s">
         <v>35</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J28" s="22"/>
-      <c r="K28" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="L28" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="M28" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="N28" s="22"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="M28" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="N28" s="16"/>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="44"/>
+      <c r="C29" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="56">
+        <v>103886</v>
+      </c>
+      <c r="E29" s="56"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="32"/>
       <c r="H29" s="1" t="s">
         <v>36</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J29" s="22"/>
-      <c r="K29" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="L29" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="M29" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="N29" s="22"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="M29" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="N29" s="16"/>
     </row>
     <row r="30" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="44"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="32"/>
       <c r="H30" s="1" t="s">
         <v>37</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J30" s="22"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="M30" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="N30" s="22"/>
-      <c r="O30" s="55"/>
-      <c r="P30" s="55"/>
-      <c r="Q30" s="55"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="M30" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="N30" s="16"/>
+      <c r="O30" s="41"/>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="41"/>
     </row>
     <row r="31" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C31" s="66" t="s">
-        <v>88</v>
-      </c>
-      <c r="D31" s="34">
-        <v>103886</v>
-      </c>
-      <c r="E31" s="34"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="44"/>
+      <c r="C31"/>
+      <c r="D31" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="59"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="32"/>
       <c r="H31" s="1" t="s">
         <v>38</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J31" s="56"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="M31" s="23" t="s">
+      <c r="J31" s="42"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M31" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="N31" s="15"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+    </row>
+    <row r="32" spans="3:17" ht="21" x14ac:dyDescent="0.4">
+      <c r="C32" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="43"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I32" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="N31" s="21"/>
-      <c r="O31" s="22"/>
-      <c r="P31" s="22"/>
-      <c r="Q31" s="22"/>
-    </row>
-    <row r="32" spans="3:17" ht="21" x14ac:dyDescent="0.4">
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="I32" s="23" t="s">
+      <c r="J32" s="43"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="M32" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="N32" s="40"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
+    </row>
+    <row r="33" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C33" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="34"/>
+      <c r="G33" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="H33" s="56">
+        <v>99224</v>
+      </c>
+      <c r="I33" s="56"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="M33" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="J32" s="57"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="M32" s="23" t="s">
+      <c r="N33" s="37"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+    </row>
+    <row r="34" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C34" s="2"/>
+      <c r="D34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N32" s="54"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="22"/>
-      <c r="Q32" s="22"/>
-    </row>
-    <row r="33" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C33"/>
-      <c r="D33" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="E33" s="33"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="66" t="s">
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="M34" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="N34" s="37"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+    </row>
+    <row r="35" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C35" s="3"/>
+      <c r="D35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="I35" s="59"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="H33" s="34">
-        <v>99224</v>
-      </c>
-      <c r="I33" s="34"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="M33" s="23" t="s">
+      <c r="L35" s="56">
+        <v>15</v>
+      </c>
+      <c r="M35" s="56"/>
+      <c r="N35" s="37"/>
+      <c r="O35" s="42"/>
+      <c r="P35" s="42"/>
+      <c r="Q35" s="42"/>
+    </row>
+    <row r="36" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C36" s="3"/>
+      <c r="D36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="N33" s="51"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="22"/>
-      <c r="Q33" s="22"/>
-    </row>
-    <row r="34" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C34" s="12" t="s">
+      <c r="F36" s="46"/>
+      <c r="G36" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="H36" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="I36" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="M34" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="N34" s="51"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
-      <c r="Q34" s="22"/>
-    </row>
-    <row r="35" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C35" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="I35" s="16"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="M35" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="N35" s="51"/>
-      <c r="O35" s="56"/>
-      <c r="P35" s="56"/>
-      <c r="Q35" s="56"/>
-    </row>
-    <row r="36" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C36" s="2"/>
-      <c r="D36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F36" s="60"/>
-      <c r="G36" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="H36" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="I36" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="J36" s="48"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="M36" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="N36" s="51"/>
-      <c r="O36" s="22"/>
-      <c r="P36" s="22"/>
-      <c r="Q36" s="22"/>
+      <c r="N36" s="37"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
     </row>
     <row r="37" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C37" s="3"/>
+      <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F37" s="60"/>
-      <c r="G37" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" s="46"/>
+      <c r="G37" s="29" t="s">
         <v>73</v>
       </c>
       <c r="H37" s="1" t="s">
@@ -2104,301 +2074,280 @@
       <c r="I37" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J37" s="48"/>
-      <c r="K37" s="66" t="s">
-        <v>88</v>
-      </c>
-      <c r="L37" s="34">
-        <v>15</v>
-      </c>
-      <c r="M37" s="34"/>
-      <c r="N37" s="51"/>
-      <c r="O37" s="22"/>
-      <c r="P37" s="22"/>
-      <c r="Q37" s="22"/>
+      <c r="N37" s="37"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="16"/>
     </row>
     <row r="38" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C38" s="3"/>
-      <c r="D38" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E38" s="39" t="s">
+      <c r="C38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="F38" s="48"/>
-      <c r="G38" s="44"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="32"/>
       <c r="H38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O38" s="22"/>
-      <c r="P38" s="22"/>
-      <c r="Q38" s="22"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="M38" s="59"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
     </row>
     <row r="39" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E39" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="F39" s="48"/>
-      <c r="G39" s="44"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="32"/>
       <c r="H39" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O39" s="21"/>
-      <c r="P39" s="21"/>
-      <c r="Q39" s="21"/>
+      <c r="K39" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="L39" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="M39" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
+      <c r="Q39" s="15"/>
     </row>
     <row r="40" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E40" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="F40" s="48"/>
-      <c r="G40" s="44"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="32"/>
       <c r="H40" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="K40" s="5"/>
-      <c r="L40" s="33" t="s">
+      <c r="K40" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="L40" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="M40" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="15"/>
+    </row>
+    <row r="41" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C41" s="48"/>
+      <c r="D41" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" s="34"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="I41" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="K41" s="9"/>
+      <c r="L41" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="M40" s="33"/>
-      <c r="O40" s="21"/>
-      <c r="P40" s="21"/>
-      <c r="Q40" s="21"/>
-    </row>
-    <row r="41" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C41" s="1"/>
-      <c r="D41" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="39" t="s">
+      <c r="M41" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="O41" s="43"/>
+      <c r="P41" s="43"/>
+      <c r="Q41" s="43"/>
+    </row>
+    <row r="42" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C42" s="4"/>
+      <c r="D42" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F41" s="48"/>
-      <c r="G41" s="64"/>
-      <c r="H41" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="I41" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="K41" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="L41" s="58" t="s">
-        <v>54</v>
-      </c>
-      <c r="M41" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="O41" s="57"/>
-      <c r="P41" s="57"/>
-      <c r="Q41" s="57"/>
-    </row>
-    <row r="42" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C42" s="1"/>
-      <c r="D42" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E42" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="F42" s="48"/>
+      <c r="F42" s="34"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-      <c r="K42" s="59" t="s">
-        <v>73</v>
-      </c>
-      <c r="L42" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="M42" s="23" t="s">
+      <c r="K42" s="9"/>
+      <c r="L42" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="M42" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+      <c r="Q42" s="16"/>
+    </row>
+    <row r="43" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C43" s="1"/>
+      <c r="D43" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F43" s="34"/>
+      <c r="G43" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="H43" s="56">
+        <v>19015</v>
+      </c>
+      <c r="I43" s="56"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="M43" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="O43" s="16"/>
+      <c r="P43" s="16"/>
+      <c r="Q43" s="16"/>
+    </row>
+    <row r="44" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C44" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E44" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="O42" s="22"/>
-      <c r="P42" s="22"/>
-      <c r="Q42" s="22"/>
-    </row>
-    <row r="43" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C43" s="62"/>
-      <c r="D43" s="62" t="s">
-        <v>19</v>
-      </c>
-      <c r="E43" s="63" t="s">
-        <v>56</v>
-      </c>
-      <c r="F43" s="48"/>
-      <c r="G43" s="66" t="s">
-        <v>88</v>
-      </c>
-      <c r="H43" s="34">
-        <v>19015</v>
-      </c>
-      <c r="I43" s="34"/>
-      <c r="K43" s="9"/>
-      <c r="L43" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="M43" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="O43" s="22"/>
-      <c r="P43" s="22"/>
-      <c r="Q43" s="22"/>
-    </row>
-    <row r="44" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C44" s="4"/>
-      <c r="D44" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
       <c r="K44" s="9"/>
       <c r="L44" s="23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="M44" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="O44" s="22"/>
-      <c r="P44" s="22"/>
-      <c r="Q44" s="22"/>
+        <v>59</v>
+      </c>
+      <c r="O44" s="16"/>
+      <c r="P44" s="16"/>
+      <c r="Q44" s="16"/>
     </row>
     <row r="45" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C45" s="1"/>
-      <c r="D45" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="E45" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="F45" s="22"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
-      <c r="K45" s="10"/>
-      <c r="L45" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="M45" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="N45" s="22"/>
-      <c r="O45" s="22"/>
-      <c r="P45" s="22"/>
-      <c r="Q45" s="22"/>
+      <c r="C45" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" s="56">
+        <v>32951</v>
+      </c>
+      <c r="E45" s="56"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="L45" s="56">
+        <v>5</v>
+      </c>
+      <c r="M45" s="56"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="16"/>
+      <c r="P45" s="16"/>
+      <c r="Q45" s="16"/>
     </row>
     <row r="46" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C46" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D46" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="E46" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="F46" s="22"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="M46" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="N46" s="22"/>
-      <c r="O46" s="22"/>
-      <c r="P46" s="22"/>
-      <c r="Q46" s="22"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="N46" s="16"/>
+      <c r="O46" s="16"/>
+      <c r="P46" s="16"/>
+      <c r="Q46" s="16"/>
     </row>
     <row r="47" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C47" s="66" t="s">
-        <v>88</v>
-      </c>
-      <c r="D47" s="34">
-        <v>32951</v>
-      </c>
-      <c r="E47" s="34"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="22"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
-      <c r="K47" s="74" t="s">
-        <v>102</v>
-      </c>
-      <c r="L47" s="34">
-        <v>5</v>
-      </c>
-      <c r="M47" s="34"/>
-      <c r="N47" s="22"/>
-      <c r="O47" s="22"/>
-      <c r="P47" s="22"/>
-      <c r="Q47" s="22"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="N47" s="16"/>
+      <c r="O47" s="16"/>
+      <c r="P47" s="16"/>
+      <c r="Q47" s="16"/>
     </row>
     <row r="48" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="F48" s="22"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="22"/>
-      <c r="J48" s="22"/>
-      <c r="N48" s="22"/>
-      <c r="O48" s="22"/>
-      <c r="P48" s="22"/>
-      <c r="Q48" s="22"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="N48" s="16"/>
+      <c r="O48" s="16"/>
+      <c r="P48" s="16"/>
+      <c r="Q48" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="H35:I35"/>
+  <mergeCells count="24">
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="L18:M18"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="L7:M7"/>
-    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D29:E29"/>
     <mergeCell ref="L16:M16"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="L23:M23"/>
     <mergeCell ref="L25:M25"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="D45:E45"/>
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="L18:M18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>